<commit_message>
* updated texts * fixed buttons in gui
</commit_message>
<xml_diff>
--- a/resources/texts.xlsx
+++ b/resources/texts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HungryChameleon\export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HungryChameleon\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>KEY</t>
   </si>
@@ -87,6 +87,33 @@
   </si>
   <si>
     <t>Настройки</t>
+  </si>
+  <si>
+    <t>STR_SHOP</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>Магазин</t>
+  </si>
+  <si>
+    <t>STR_OK</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Ладно</t>
+  </si>
+  <si>
+    <t>STR_CANCEL</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Отмена</t>
   </si>
 </sst>
 </file>
@@ -412,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +531,39 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>